<commit_message>
add initial version of target orientation
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init_test.xlsx
+++ b/run_commands/inputs/init_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBD605C-4671-4EFE-9087-A787473AB623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45DDC7C-9BB6-4F49-8AD5-8EB97656FE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>1d</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>ETH-USD</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Technical</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:G985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -445,10 +445,10 @@
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -460,7 +460,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>7</v>

</xml_diff>